<commit_message>
Added writing to JSON file
</commit_message>
<xml_diff>
--- a/target/classes/statistics.xlsx
+++ b/target/classes/statistics.xlsx
@@ -32,25 +32,25 @@
     <t>Медицина</t>
   </si>
   <si>
-    <t xml:space="preserve">nullМосковский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт, </t>
+    <t xml:space="preserve">Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт, </t>
   </si>
   <si>
     <t>Физика</t>
   </si>
   <si>
-    <t xml:space="preserve">nullМосковский Выдуманный Университет, Московский Придуманный Институт, </t>
+    <t xml:space="preserve">Московский Выдуманный Университет, Московский Придуманный Институт, </t>
   </si>
   <si>
     <t>Лингвистика</t>
   </si>
   <si>
-    <t xml:space="preserve">nullВоронежский Литературно-Переводческий Университет, </t>
+    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет, </t>
   </si>
   <si>
     <t>Математика</t>
   </si>
   <si>
-    <t xml:space="preserve">nullКазанский Университет Вычислений, </t>
+    <t xml:space="preserve">Казанский Университет Вычислений, </t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
     <col min="2" max="2" width="44.04296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="49.74609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="31.68359375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="139.88671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="136.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>